<commit_message>
Parking and Transit Modification
</commit_message>
<xml_diff>
--- a/ARCProject/ArcTest.xlsx
+++ b/ARCProject/ArcTest.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\Abhishek\ARCProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="6210" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13950" windowHeight="7110" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NewBuildingProject" sheetId="1" r:id="rId1"/>
@@ -13,15 +18,16 @@
     <sheet name="NewCommunityProject" sheetId="6" r:id="rId4"/>
     <sheet name="Payment" sheetId="2" r:id="rId5"/>
     <sheet name="Login" sheetId="3" r:id="rId6"/>
-    <sheet name="Add Meter" sheetId="4" r:id="rId7"/>
-    <sheet name="BEnergy" sheetId="7" r:id="rId8"/>
-    <sheet name="BWater" sheetId="8" r:id="rId9"/>
-    <sheet name="BWaste" sheetId="9" r:id="rId10"/>
+    <sheet name="CDataInput" sheetId="12" r:id="rId7"/>
+    <sheet name="Add Meter" sheetId="4" r:id="rId8"/>
+    <sheet name="BEnergy" sheetId="7" r:id="rId9"/>
+    <sheet name="BWater" sheetId="8" r:id="rId10"/>
+    <sheet name="BWaste" sheetId="9" r:id="rId11"/>
+    <sheet name="NewParkingProject" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F18"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="719" uniqueCount="290">
   <si>
     <t>Project Name</t>
   </si>
@@ -166,9 +172,6 @@
     <t>annual_ridership</t>
   </si>
   <si>
-    <t>200000</t>
-  </si>
-  <si>
     <t>week_opr_hrs</t>
   </si>
   <si>
@@ -187,12 +190,6 @@
     <t>45</t>
   </si>
   <si>
-    <t>Building LEED for transit</t>
-  </si>
-  <si>
-    <t>Building Parksmart</t>
-  </si>
-  <si>
     <t>Parksmart</t>
   </si>
   <si>
@@ -589,15 +586,6 @@
     <t>OwnerCountry</t>
   </si>
   <si>
-    <t>5600</t>
-  </si>
-  <si>
-    <t>4500</t>
-  </si>
-  <si>
-    <t>3388</t>
-  </si>
-  <si>
     <t>56211</t>
   </si>
   <si>
@@ -607,30 +595,15 @@
     <t>Chicago</t>
   </si>
   <si>
-    <t>LEEDCitiesTestProject 11092</t>
-  </si>
-  <si>
     <t>editArea</t>
   </si>
   <si>
     <t>editPopulation</t>
   </si>
   <si>
-    <t>4000</t>
-  </si>
-  <si>
     <t>18000</t>
   </si>
   <si>
-    <t>6553</t>
-  </si>
-  <si>
-    <t>3256</t>
-  </si>
-  <si>
-    <t>1623</t>
-  </si>
-  <si>
     <t>P &amp; C Construction, Inc.</t>
   </si>
   <si>
@@ -670,21 +643,12 @@
     <t>$ 1500.00</t>
   </si>
   <si>
-    <t>US Building LEED v4 138984</t>
-  </si>
-  <si>
     <t>US Building None 382094</t>
   </si>
   <si>
     <t>US Building Other 271067</t>
   </si>
   <si>
-    <t>CitiesNone 89625</t>
-  </si>
-  <si>
-    <t>CitiesOther 333362</t>
-  </si>
-  <si>
     <t>CommunityLeed 35133</t>
   </si>
   <si>
@@ -694,23 +658,263 @@
     <t>CommunityNone 593800</t>
   </si>
   <si>
-    <t>US Building LEED v4 273685</t>
-  </si>
-  <si>
-    <t>US Building LEED v4 329983</t>
-  </si>
-  <si>
-    <t>US Building LEED v4 622311</t>
+    <t>US Building LEED v4 355214</t>
+  </si>
+  <si>
+    <t>TONS</t>
+  </si>
+  <si>
+    <t>LBS</t>
+  </si>
+  <si>
+    <t>KBTU</t>
+  </si>
+  <si>
+    <t>MTCO2e</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>ADeatailsUnitReading5</t>
+  </si>
+  <si>
+    <t>ADeatailsUnitReading4</t>
+  </si>
+  <si>
+    <t>ADeatailsUnitReading3</t>
+  </si>
+  <si>
+    <t>ADeatailsUnitReading2</t>
+  </si>
+  <si>
+    <t>ADeatailsUnitReading1</t>
+  </si>
+  <si>
+    <t>ADeatailsValueReading5</t>
+  </si>
+  <si>
+    <t>ADeatailsValueReading4</t>
+  </si>
+  <si>
+    <t>ADeatailsValueReading3</t>
+  </si>
+  <si>
+    <t>ADeatailsValueReading2</t>
+  </si>
+  <si>
+    <t>ADeatailsValueReading1</t>
+  </si>
+  <si>
+    <t>HPReading5</t>
+  </si>
+  <si>
+    <t>HPReading4</t>
+  </si>
+  <si>
+    <t>HPReading3</t>
+  </si>
+  <si>
+    <t>HPReading2</t>
+  </si>
+  <si>
+    <t>HPReading1</t>
+  </si>
+  <si>
+    <t>TReading5</t>
+  </si>
+  <si>
+    <t>TReading4</t>
+  </si>
+  <si>
+    <t>TReading3</t>
+  </si>
+  <si>
+    <t>TReading2</t>
+  </si>
+  <si>
+    <t>TReading1</t>
+  </si>
+  <si>
+    <t>wastediversion5</t>
+  </si>
+  <si>
+    <t>wastediversion4</t>
+  </si>
+  <si>
+    <t>wastediversion3</t>
+  </si>
+  <si>
+    <t>wastediversion2</t>
+  </si>
+  <si>
+    <t>wastediversion1</t>
+  </si>
+  <si>
+    <t>wastegeneration5</t>
+  </si>
+  <si>
+    <t>wastegeneration4</t>
+  </si>
+  <si>
+    <t>wastegeneration3</t>
+  </si>
+  <si>
+    <t>wastegeneration2</t>
+  </si>
+  <si>
+    <t>wastegeneration1</t>
+  </si>
+  <si>
+    <t>WaterReading5</t>
+  </si>
+  <si>
+    <t>WaterReading4</t>
+  </si>
+  <si>
+    <t>WaterReading3</t>
+  </si>
+  <si>
+    <t>WaterReading2</t>
+  </si>
+  <si>
+    <t>WaterReading1</t>
+  </si>
+  <si>
+    <t>EReading5</t>
+  </si>
+  <si>
+    <t>EReading4</t>
+  </si>
+  <si>
+    <t>EReading3</t>
+  </si>
+  <si>
+    <t>EReading2</t>
+  </si>
+  <si>
+    <t>EReading1</t>
+  </si>
+  <si>
+    <t>Parking Spaces</t>
+  </si>
+  <si>
+    <t>parking structure</t>
+  </si>
+  <si>
+    <t>Data Commisioned</t>
+  </si>
+  <si>
+    <t>parkDetail</t>
+  </si>
+  <si>
+    <t>US Building Parking 346951</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>2015-02-04</t>
+  </si>
+  <si>
+    <t>2101 L St NW #500</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>20037</t>
+  </si>
+  <si>
+    <t>http://www.parking-net.com</t>
+  </si>
+  <si>
+    <t>When assigned parking is provided, designated accessible parking .</t>
+  </si>
+  <si>
+    <t>US Building Parking 322031</t>
+  </si>
+  <si>
+    <t>CitiesLeed 386677</t>
+  </si>
+  <si>
+    <t>CitiesNone 309844</t>
+  </si>
+  <si>
+    <t>CitiesOther 492610</t>
+  </si>
+  <si>
+    <t>TFulltimestaff</t>
+  </si>
+  <si>
+    <t>TWeeklyOperatinghours</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>US Building Aboveground 704159</t>
+  </si>
+  <si>
+    <t>TMAnnualRidership</t>
+  </si>
+  <si>
+    <t>TAveragetime</t>
+  </si>
+  <si>
+    <t>365</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>US Building Parking 663471</t>
+  </si>
+  <si>
+    <t>655</t>
+  </si>
+  <si>
+    <t>325</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>560</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>338</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -736,13 +940,69 @@
       <color indexed="16"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -758,7 +1018,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -771,12 +1031,40 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1052,42 +1340,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD6"/>
+  <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="25.70703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="9" max="9" style="2" width="9.140625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="14" max="14" style="2" width="9.140625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="5" width="12.140625" collapsed="true"/>
-    <col min="16" max="17" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="9.80078125" collapsed="true"/>
-    <col min="29" max="29" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="1" max="1" width="33.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="2" collapsed="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.140625" style="2" collapsed="1"/>
+    <col min="15" max="15" width="12.140625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="19" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="16.140625" customWidth="1"/>
+    <col min="32" max="32" width="16" customWidth="1"/>
+    <col min="33" max="33" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1389,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1137,51 +1428,63 @@
         <v>42</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>44</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>30</v>
       </c>
       <c r="AC1" s="2" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="AD1" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>273</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
@@ -1196,13 +1499,13 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>28</v>
@@ -1214,33 +1517,33 @@
         <v>31</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="M2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O2" s="6" t="s">
         <v>32</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AB2" s="11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>52</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>277</v>
       </c>
       <c r="B3" t="s">
         <v>13</v>
@@ -1255,7 +1558,7 @@
         <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>17</v>
@@ -1279,193 +1582,205 @@
         <v>41</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="P3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Q3" t="s">
         <v>43</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>45</v>
+        <v>275</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+      <c r="AE3" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="AF3" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AG3" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="AH3" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>261</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="V4" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="L4" t="s">
-        <v>56</v>
-      </c>
-      <c r="M4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="W4" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="AB4" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>195</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>203</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>206</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>215</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
       </c>
       <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" t="s">
         <v>66</v>
       </c>
-      <c r="D5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E5" t="s">
-        <v>69</v>
-      </c>
       <c r="F5" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="M5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L5" s="2" t="s">
+      <c r="N5" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="M5" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="Y5" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AB5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D6" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F6" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="J6" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="N6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="L6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="Y6" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="Z6" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="AB6" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -1482,6 +1797,167 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -1490,211 +1966,582 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="12.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" t="s">
         <v>149</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>150</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>151</v>
       </c>
-      <c r="F1" t="s">
-        <v>152</v>
-      </c>
-      <c r="G1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>154</v>
       </c>
-      <c r="I1" t="s">
-        <v>157</v>
-      </c>
       <c r="J1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="G2" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="J2" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="E3" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="G3" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H3" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="J3" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="E4" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="G4" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="E5" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H5" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="J5" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="E6" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>143</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>159</v>
-      </c>
       <c r="J6" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="P1" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="P2" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M4" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="P5" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="J6" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="J7" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="O7" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="P7" s="12" t="s">
+        <v>268</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:V7">
+    <cfRule type="uniqueValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1709,37 +2556,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="1" max="1" width="19.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1758,51 +2605,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="24.5703125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="11" max="12" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
-      </c>
-      <c r="E1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G1" t="s">
-        <v>185</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -1823,10 +2670,10 @@
         <v>29</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>30</v>
@@ -1838,159 +2685,159 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>216</v>
+      <c r="A2" s="24" t="s">
+        <v>270</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>186</v>
+        <v>287</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L2" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="R2" t="s">
         <v>190</v>
       </c>
-      <c r="K2" t="s">
-        <v>191</v>
-      </c>
-      <c r="L2" t="s">
-        <v>56</v>
-      </c>
-      <c r="M2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="R2" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>217</v>
+      <c r="A3" s="24" t="s">
+        <v>272</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>187</v>
+        <v>288</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" t="s">
         <v>92</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="K3" t="s">
+      <c r="P3" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="R3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4" t="s">
         <v>94</v>
       </c>
-      <c r="L3" t="s">
-        <v>72</v>
-      </c>
-      <c r="M3" t="s">
-        <v>95</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="R3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>192</v>
-      </c>
-      <c r="B4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" t="s">
-        <v>97</v>
-      </c>
       <c r="E4" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H4" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="J4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" t="s">
+        <v>99</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="J4" t="s">
-        <v>100</v>
-      </c>
-      <c r="K4" t="s">
-        <v>101</v>
-      </c>
-      <c r="L4" t="s">
-        <v>82</v>
-      </c>
-      <c r="M4" t="s">
-        <v>102</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2008,55 +2855,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="11" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="10.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
         <v>179</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>180</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>181</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>182</v>
-      </c>
-      <c r="E1" t="s">
-        <v>183</v>
-      </c>
-      <c r="F1" t="s">
-        <v>184</v>
-      </c>
-      <c r="G1" t="s">
-        <v>185</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -2077,10 +2924,10 @@
         <v>29</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>30</v>
@@ -2093,161 +2940,161 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>197</v>
+        <v>283</v>
       </c>
       <c r="I2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="J2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K2" t="s">
-        <v>101</v>
-      </c>
-      <c r="L2" t="s">
-        <v>82</v>
-      </c>
-      <c r="M2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>109</v>
-      </c>
       <c r="P2" s="4" t="s">
-        <v>195</v>
+        <v>286</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>198</v>
+        <v>284</v>
       </c>
       <c r="I3" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="J3" t="s">
+        <v>108</v>
+      </c>
+      <c r="K3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M3" t="s">
+        <v>109</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="J3" t="s">
-        <v>111</v>
-      </c>
-      <c r="K3" t="s">
-        <v>112</v>
-      </c>
-      <c r="L3" t="s">
-        <v>56</v>
-      </c>
-      <c r="M3" t="s">
-        <v>112</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="P3" s="4" t="s">
-        <v>195</v>
+        <v>286</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>199</v>
+        <v>285</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J4" t="s">
+        <v>113</v>
+      </c>
+      <c r="K4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" t="s">
         <v>115</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="K4" t="s">
-        <v>117</v>
-      </c>
-      <c r="L4" t="s">
-        <v>72</v>
-      </c>
-      <c r="M4" t="s">
-        <v>118</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>119</v>
-      </c>
       <c r="P4" s="4" t="s">
-        <v>195</v>
+        <v>286</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -2265,37 +3112,37 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="3" max="5" customWidth="true" width="15.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="5" width="13.5703125" collapsed="true"/>
+    <col min="1" max="2" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="5" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.5703125" style="5" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" t="s">
         <v>126</v>
       </c>
-      <c r="B1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D1" t="s">
-        <v>129</v>
-      </c>
       <c r="E1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F1" t="s">
         <v>18</v>
@@ -2322,24 +3169,24 @@
         <v>30</v>
       </c>
       <c r="N1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -2351,37 +3198,37 @@
         <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M2" s="9"/>
       <c r="N2" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -2393,37 +3240,37 @@
         <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M3" s="9"/>
       <c r="N3" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -2435,37 +3282,37 @@
         <v>22</v>
       </c>
       <c r="I4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M4" s="9"/>
       <c r="N4" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -2477,37 +3324,37 @@
         <v>22</v>
       </c>
       <c r="I5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M5" s="9"/>
       <c r="N5" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -2519,20 +3366,20 @@
         <v>22</v>
       </c>
       <c r="I6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K6" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="M6" s="9"/>
       <c r="N6" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -2558,12 +3405,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="1" max="1" width="19.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
@@ -2571,42 +3418,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2615,6 +3462,646 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AO5"/>
+  <sheetViews>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="20.140625" customWidth="1"/>
+    <col min="32" max="32" width="24.5703125" customWidth="1"/>
+    <col min="33" max="33" width="26" customWidth="1"/>
+    <col min="41" max="41" width="15.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="L1" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="P1" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q1" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="R1" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="S1" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="T1" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>236</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>235</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>232</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="AA1" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="AB1" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC1" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD1" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>226</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="AJ1" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="AK1" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="AL1" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="AM1" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="AN1" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="AO1" s="14"/>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.98</v>
+      </c>
+      <c r="B2">
+        <v>0.66</v>
+      </c>
+      <c r="C2">
+        <v>1.22</v>
+      </c>
+      <c r="D2">
+        <v>0.99</v>
+      </c>
+      <c r="E2">
+        <v>0.33</v>
+      </c>
+      <c r="F2">
+        <v>0.98</v>
+      </c>
+      <c r="G2">
+        <v>0.66</v>
+      </c>
+      <c r="H2">
+        <v>1.22</v>
+      </c>
+      <c r="I2">
+        <v>0.99</v>
+      </c>
+      <c r="J2">
+        <v>0.33</v>
+      </c>
+      <c r="K2">
+        <v>0.98</v>
+      </c>
+      <c r="L2">
+        <v>0.66</v>
+      </c>
+      <c r="M2">
+        <v>1.22</v>
+      </c>
+      <c r="N2">
+        <v>0.99</v>
+      </c>
+      <c r="O2">
+        <v>0.33</v>
+      </c>
+      <c r="P2">
+        <v>0.98</v>
+      </c>
+      <c r="Q2">
+        <v>0.66</v>
+      </c>
+      <c r="R2">
+        <v>1.22</v>
+      </c>
+      <c r="S2">
+        <v>0.99</v>
+      </c>
+      <c r="T2">
+        <v>0.33</v>
+      </c>
+      <c r="U2" s="13">
+        <v>22</v>
+      </c>
+      <c r="V2" s="13">
+        <v>34</v>
+      </c>
+      <c r="W2" s="13">
+        <v>53</v>
+      </c>
+      <c r="X2" s="13">
+        <v>34</v>
+      </c>
+      <c r="Y2" s="13">
+        <v>34</v>
+      </c>
+      <c r="Z2" s="13">
+        <v>43</v>
+      </c>
+      <c r="AA2" s="13">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="13">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="13">
+        <v>22</v>
+      </c>
+      <c r="AD2" s="13">
+        <v>22</v>
+      </c>
+      <c r="AE2" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF2" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="AG2" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH2" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="AI2" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ2" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK2" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AM2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN2" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.98</v>
+      </c>
+      <c r="B3">
+        <v>0.66</v>
+      </c>
+      <c r="C3">
+        <v>1.22</v>
+      </c>
+      <c r="D3">
+        <v>0.99</v>
+      </c>
+      <c r="E3">
+        <v>0.33</v>
+      </c>
+      <c r="F3">
+        <v>0.98</v>
+      </c>
+      <c r="G3">
+        <v>0.66</v>
+      </c>
+      <c r="H3">
+        <v>1.22</v>
+      </c>
+      <c r="I3">
+        <v>0.99</v>
+      </c>
+      <c r="J3">
+        <v>0.33</v>
+      </c>
+      <c r="K3">
+        <v>0.98</v>
+      </c>
+      <c r="L3">
+        <v>0.66</v>
+      </c>
+      <c r="M3">
+        <v>1.22</v>
+      </c>
+      <c r="N3">
+        <v>0.99</v>
+      </c>
+      <c r="O3">
+        <v>0.33</v>
+      </c>
+      <c r="P3">
+        <v>0.98</v>
+      </c>
+      <c r="Q3">
+        <v>0.66</v>
+      </c>
+      <c r="R3">
+        <v>1.22</v>
+      </c>
+      <c r="S3">
+        <v>0.99</v>
+      </c>
+      <c r="T3">
+        <v>0.33</v>
+      </c>
+      <c r="U3" s="13">
+        <v>22</v>
+      </c>
+      <c r="V3" s="13">
+        <v>34</v>
+      </c>
+      <c r="W3" s="13">
+        <v>53</v>
+      </c>
+      <c r="X3" s="13">
+        <v>34</v>
+      </c>
+      <c r="Y3" s="13">
+        <v>34</v>
+      </c>
+      <c r="Z3" s="13">
+        <v>43</v>
+      </c>
+      <c r="AA3" s="13">
+        <v>32</v>
+      </c>
+      <c r="AB3" s="13">
+        <v>33</v>
+      </c>
+      <c r="AC3" s="13">
+        <v>22</v>
+      </c>
+      <c r="AD3" s="13">
+        <v>22</v>
+      </c>
+      <c r="AE3" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF3" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="AG3" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH3" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="AI3" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN3" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.98</v>
+      </c>
+      <c r="B4">
+        <v>0.66</v>
+      </c>
+      <c r="C4">
+        <v>1.22</v>
+      </c>
+      <c r="D4">
+        <v>0.99</v>
+      </c>
+      <c r="E4">
+        <v>0.33</v>
+      </c>
+      <c r="F4">
+        <v>0.98</v>
+      </c>
+      <c r="G4">
+        <v>0.66</v>
+      </c>
+      <c r="H4">
+        <v>1.22</v>
+      </c>
+      <c r="I4">
+        <v>0.99</v>
+      </c>
+      <c r="J4">
+        <v>0.33</v>
+      </c>
+      <c r="K4">
+        <v>0.98</v>
+      </c>
+      <c r="L4">
+        <v>0.66</v>
+      </c>
+      <c r="M4">
+        <v>1.22</v>
+      </c>
+      <c r="N4">
+        <v>0.99</v>
+      </c>
+      <c r="O4">
+        <v>0.33</v>
+      </c>
+      <c r="P4">
+        <v>0.98</v>
+      </c>
+      <c r="Q4">
+        <v>0.66</v>
+      </c>
+      <c r="R4">
+        <v>1.22</v>
+      </c>
+      <c r="S4">
+        <v>0.99</v>
+      </c>
+      <c r="T4">
+        <v>0.33</v>
+      </c>
+      <c r="U4" s="13">
+        <v>22</v>
+      </c>
+      <c r="V4" s="13">
+        <v>34</v>
+      </c>
+      <c r="W4" s="13">
+        <v>53</v>
+      </c>
+      <c r="X4" s="13">
+        <v>34</v>
+      </c>
+      <c r="Y4" s="13">
+        <v>34</v>
+      </c>
+      <c r="Z4" s="13">
+        <v>43</v>
+      </c>
+      <c r="AA4" s="13">
+        <v>32</v>
+      </c>
+      <c r="AB4" s="13">
+        <v>33</v>
+      </c>
+      <c r="AC4" s="13">
+        <v>22</v>
+      </c>
+      <c r="AD4" s="13">
+        <v>22</v>
+      </c>
+      <c r="AE4" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF4" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="AG4" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH4" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="AI4" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ4" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK4" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="AL4" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AM4" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN4" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.98</v>
+      </c>
+      <c r="B5">
+        <v>0.66</v>
+      </c>
+      <c r="C5">
+        <v>1.22</v>
+      </c>
+      <c r="D5">
+        <v>0.99</v>
+      </c>
+      <c r="E5">
+        <v>0.33</v>
+      </c>
+      <c r="F5">
+        <v>0.98</v>
+      </c>
+      <c r="G5">
+        <v>0.66</v>
+      </c>
+      <c r="H5">
+        <v>1.22</v>
+      </c>
+      <c r="I5">
+        <v>0.99</v>
+      </c>
+      <c r="J5">
+        <v>0.33</v>
+      </c>
+      <c r="K5">
+        <v>0.98</v>
+      </c>
+      <c r="L5">
+        <v>0.66</v>
+      </c>
+      <c r="M5">
+        <v>1.22</v>
+      </c>
+      <c r="N5">
+        <v>0.99</v>
+      </c>
+      <c r="O5">
+        <v>0.33</v>
+      </c>
+      <c r="P5">
+        <v>0.98</v>
+      </c>
+      <c r="Q5">
+        <v>0.66</v>
+      </c>
+      <c r="R5">
+        <v>1.22</v>
+      </c>
+      <c r="S5">
+        <v>0.99</v>
+      </c>
+      <c r="T5">
+        <v>0.33</v>
+      </c>
+      <c r="U5" s="13">
+        <v>22</v>
+      </c>
+      <c r="V5" s="13">
+        <v>34</v>
+      </c>
+      <c r="W5" s="13">
+        <v>53</v>
+      </c>
+      <c r="X5" s="13">
+        <v>34</v>
+      </c>
+      <c r="Y5" s="13">
+        <v>34</v>
+      </c>
+      <c r="Z5" s="13">
+        <v>43</v>
+      </c>
+      <c r="AA5" s="13">
+        <v>32</v>
+      </c>
+      <c r="AB5" s="13">
+        <v>33</v>
+      </c>
+      <c r="AC5" s="13">
+        <v>22</v>
+      </c>
+      <c r="AD5" s="13">
+        <v>22</v>
+      </c>
+      <c r="AE5" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="AF5" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="AG5" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH5" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="AI5" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="AJ5" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK5" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="AL5" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="AM5" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="AN5" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2624,8 +4111,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="1" max="1" width="14" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2682,7 +4169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
@@ -2692,10 +4179,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2703,316 +4190,155 @@
         <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" t="s">
         <v>144</v>
-      </c>
-      <c r="F1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="G2" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="G3" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="G4" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="B6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="G6" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.5703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F1" t="s">
-        <v>146</v>
-      </c>
-      <c r="G1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>148</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>